<commit_message>
added defaultpath, solution details
</commit_message>
<xml_diff>
--- a/Simulation/Work/data/building.xlsx
+++ b/Simulation/Work/data/building.xlsx
@@ -497,7 +497,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,8 +521,7 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <f>360*4</f>
-        <v>1440</v>
+        <v>1600</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -583,7 +582,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G9"/>
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>